<commit_message>
Specimen array sheet updated. Author - Sarita Patel
SVN-Revision: 25362
</commit_message>
<xml_diff>
--- a/TestCases/ToBeAutomated/SpecimenArray.xlsx
+++ b/TestCases/ToBeAutomated/SpecimenArray.xlsx
@@ -216,18 +216,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Test to ensure that user is able to add Tissue speicmen Array successfully using label (Auto allocation)</t>
-  </si>
-  <si>
-    <t>Test to ensure that user is able to add Cell Specimen Array successfully using label  (Auto allocation)</t>
-  </si>
-  <si>
-    <t>Test to ensure that user is able to add Fluid Specimen array successsfully using label  (Auto allocation)</t>
-  </si>
-  <si>
-    <t>Test to ensure that user is able to add Molecular specimen array successfully using label  (Auto allocation)</t>
-  </si>
-  <si>
     <t>Test to ensure that user is able to add Tissue speicmen Array successfully using bode (Manual allocation)</t>
   </si>
   <si>
@@ -247,6 +235,18 @@
   </si>
   <si>
     <t>Test to ensure that activity status can be updated from active to disabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test to ensure that user is able to add Tissue speicmen Array successfully using label </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test to ensure that user is able to add Cell Specimen Array successfully using label  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test to ensure that user is able to add Fluid Specimen array successsfully using label  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test to ensure that user is able to add Molecular specimen array successfully using label </t>
   </si>
 </sst>
 </file>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CL75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:A75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -679,7 +679,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
         <v>51</v>
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -701,7 +701,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
@@ -712,7 +712,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>51</v>
@@ -723,7 +723,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
         <v>52</v>
@@ -734,7 +734,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -745,7 +745,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -756,7 +756,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:90" s="6" customFormat="1">
@@ -1031,7 +1031,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="3" customFormat="1">
@@ -1157,7 +1157,7 @@
         <v>50</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="3" customFormat="1">

</xml_diff>

<commit_message>
Edit Specimen array test case added - their status updated
SVN-Revision: 25376
</commit_message>
<xml_diff>
--- a/TestCases/ToBeAutomated/SpecimenArray.xlsx
+++ b/TestCases/ToBeAutomated/SpecimenArray.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
   <si>
     <t>Add Success</t>
   </si>
@@ -253,6 +253,15 @@
   </si>
   <si>
     <t>custom user</t>
+  </si>
+  <si>
+    <t>Edit baseed on ID</t>
+  </si>
+  <si>
+    <t>No such field exist</t>
+  </si>
+  <si>
+    <t>technician</t>
   </si>
 </sst>
 </file>
@@ -623,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CL72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1319,7 +1328,13 @@
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="G42" t="s">
+        <v>60</v>
+      </c>
+      <c r="H42" s="9">
+        <v>40610</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="30">
@@ -1333,7 +1348,13 @@
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="G43" t="s">
+        <v>60</v>
+      </c>
+      <c r="H43" s="9">
+        <v>40610</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="30">
@@ -1349,6 +1370,12 @@
       <c r="E44" t="s">
         <v>40</v>
       </c>
+      <c r="G44" t="s">
+        <v>60</v>
+      </c>
+      <c r="H44" s="9">
+        <v>40610</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="30">
       <c r="A45">
@@ -1358,10 +1385,16 @@
         <v>34</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="E45" t="s">
         <v>40</v>
+      </c>
+      <c r="G45" t="s">
+        <v>60</v>
+      </c>
+      <c r="H45" s="9">
+        <v>40610</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1377,6 +1410,12 @@
       <c r="E46" t="s">
         <v>40</v>
       </c>
+      <c r="G46" t="s">
+        <v>60</v>
+      </c>
+      <c r="H46" s="9">
+        <v>40610</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47">
@@ -1389,8 +1428,12 @@
         <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>40</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="G47" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48">
@@ -1403,10 +1446,16 @@
         <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>40</v>
+      </c>
+      <c r="G48" t="s">
+        <v>60</v>
+      </c>
+      <c r="H48" s="9">
+        <v>40610</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>46</v>
       </c>
@@ -1417,21 +1466,30 @@
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30">
+        <v>40</v>
+      </c>
+      <c r="G49" t="s">
+        <v>60</v>
+      </c>
+      <c r="H49" s="9">
+        <v>40610</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="30">
       <c r="A50">
         <v>47</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" s="3" customFormat="1">
+      <c r="H50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="3" customFormat="1">
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:5" ht="30">
+    <row r="52" spans="1:8" ht="30">
       <c r="A52">
         <v>48</v>
       </c>
@@ -1445,7 +1503,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30">
+    <row r="53" spans="1:8" ht="30">
       <c r="A53">
         <v>49</v>
       </c>
@@ -1456,7 +1514,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30">
+    <row r="54" spans="1:8" ht="30">
       <c r="A54">
         <v>50</v>
       </c>
@@ -1467,7 +1525,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="30">
+    <row r="55" spans="1:8" ht="30">
       <c r="A55">
         <v>51</v>
       </c>
@@ -1478,7 +1536,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="30">
+    <row r="56" spans="1:8" ht="30">
       <c r="A56">
         <v>52</v>
       </c>
@@ -1486,7 +1544,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:8" ht="30">
       <c r="A57">
         <v>53</v>
       </c>
@@ -1494,7 +1552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30">
+    <row r="58" spans="1:8" ht="30">
       <c r="A58">
         <v>54</v>
       </c>
@@ -1502,7 +1560,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="30">
+    <row r="59" spans="1:8" ht="30">
       <c r="A59">
         <v>55</v>
       </c>
@@ -1510,7 +1568,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="30">
+    <row r="60" spans="1:8" ht="30">
       <c r="A60">
         <v>56</v>
       </c>
@@ -1518,7 +1576,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="30">
+    <row r="61" spans="1:8" ht="30">
       <c r="A61">
         <v>57</v>
       </c>
@@ -1526,7 +1584,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="30">
+    <row r="62" spans="1:8" ht="30">
       <c r="A62">
         <v>58</v>
       </c>
@@ -1534,7 +1592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="30">
+    <row r="63" spans="1:8" ht="30">
       <c r="A63">
         <v>59</v>
       </c>
@@ -1542,7 +1600,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="30">
+    <row r="64" spans="1:8" ht="30">
       <c r="A64">
         <v>60</v>
       </c>

</xml_diff>